<commit_message>
Revert "Update BDD enfants.xlsx"
This reverts commit 1a7ceb99fb763fc1fa787a0d840d74ad7379241c.
</commit_message>
<xml_diff>
--- a/BDD enfants.xlsx
+++ b/BDD enfants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive\Documents\GitHub\AI_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B517EB-0EA3-42B6-A9B9-C3D119C61312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FDCF46-75BB-4EE0-B862-D7BB5D52B7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="213">
   <si>
     <t>ID</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>Nour</t>
+  </si>
+  <si>
+    <t>candy</t>
   </si>
   <si>
     <t>Cherif</t>
@@ -673,8 +676,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d\-mmm"/>
-    <numFmt numFmtId="165" formatCode="dd/mm"/>
+    <numFmt numFmtId="172" formatCode="d\-mmm"/>
+    <numFmt numFmtId="173" formatCode="dd/mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -725,10 +728,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1017,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3846,7 +3849,7 @@
         <v>122</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -3854,10 +3857,10 @@
         <v>98</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>19</v>
@@ -3883,10 +3886,10 @@
         <v>99</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>201</v>

</xml_diff>